<commit_message>
Tue Dec 24 10:53:48 AM EST 2024 ozone figures
</commit_message>
<xml_diff>
--- a/ozone/ozone_VTZP_SHAP.xlsx
+++ b/ozone/ozone_VTZP_SHAP.xlsx
@@ -455,7 +455,7 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>0.003014780398379638</v>
+        <v>0.003011558224893633</v>
       </c>
     </row>
     <row r="3">
@@ -468,7 +468,7 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>0.001402354041766674</v>
+        <v>0.001398754878081991</v>
       </c>
     </row>
     <row r="4">
@@ -481,7 +481,7 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>0.00082242076277838</v>
+        <v>0.000820595559525982</v>
       </c>
     </row>
     <row r="5">
@@ -494,7 +494,7 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>0.000383306643664837</v>
+        <v>0.000383122750296422</v>
       </c>
     </row>
     <row r="6">
@@ -507,7 +507,7 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>0.0003773280276621778</v>
+        <v>0.0003771042277510145</v>
       </c>
     </row>
     <row r="7">
@@ -520,7 +520,7 @@
         </is>
       </c>
       <c r="C7" t="n">
-        <v>0.0003286952812258875</v>
+        <v>0.0003319213207371551</v>
       </c>
     </row>
     <row r="8">
@@ -533,7 +533,7 @@
         </is>
       </c>
       <c r="C8" t="n">
-        <v>0.0002912873361415984</v>
+        <v>0.000288331681822418</v>
       </c>
     </row>
     <row r="9">
@@ -546,7 +546,7 @@
         </is>
       </c>
       <c r="C9" t="n">
-        <v>0.0002577763998449835</v>
+        <v>0.0002596796759118628</v>
       </c>
     </row>
     <row r="10">
@@ -559,7 +559,7 @@
         </is>
       </c>
       <c r="C10" t="n">
-        <v>0.0002540502087579192</v>
+        <v>0.0002525646424993941</v>
       </c>
     </row>
     <row r="11">
@@ -572,7 +572,7 @@
         </is>
       </c>
       <c r="C11" t="n">
-        <v>0.0002431697507987722</v>
+        <v>0.000247711845948128</v>
       </c>
     </row>
     <row r="12">
@@ -585,7 +585,7 @@
         </is>
       </c>
       <c r="C12" t="n">
-        <v>0.0002203386198261743</v>
+        <v>0.0002170963448423999</v>
       </c>
     </row>
     <row r="13">
@@ -598,7 +598,7 @@
         </is>
       </c>
       <c r="C13" t="n">
-        <v>0.0002095416825163232</v>
+        <v>0.0002128087062505255</v>
       </c>
     </row>
     <row r="14">
@@ -611,7 +611,7 @@
         </is>
       </c>
       <c r="C14" t="n">
-        <v>0.0002054315862976648</v>
+        <v>0.0002049321912411723</v>
       </c>
     </row>
     <row r="15">
@@ -624,7 +624,7 @@
         </is>
       </c>
       <c r="C15" t="n">
-        <v>0.0001935500799616494</v>
+        <v>0.0001949469292711607</v>
       </c>
     </row>
     <row r="16">
@@ -637,33 +637,33 @@
         </is>
       </c>
       <c r="C16" t="n">
-        <v>0.0001485704347209281</v>
+        <v>0.0001489704927518552</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="1" t="n">
-        <v>34</v>
+        <v>54</v>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>$F_{q}$</t>
+          <t>$(F_{p})_{2}$</t>
         </is>
       </c>
       <c r="C17" t="n">
-        <v>0.0001376852125710126</v>
+        <v>0.0001369315222491405</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="1" t="n">
-        <v>54</v>
+        <v>34</v>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>$(F_{p})_{2}$</t>
+          <t>$F_{q}$</t>
         </is>
       </c>
       <c r="C18" t="n">
-        <v>0.000137273856336229</v>
+        <v>0.0001367220880664417</v>
       </c>
     </row>
     <row r="19">
@@ -676,7 +676,7 @@
         </is>
       </c>
       <c r="C19" t="n">
-        <v>0.0001264911677510234</v>
+        <v>0.000126689855998245</v>
       </c>
     </row>
     <row r="20">
@@ -689,7 +689,7 @@
         </is>
       </c>
       <c r="C20" t="n">
-        <v>0.0001131794881260554</v>
+        <v>0.0001139853583913129</v>
       </c>
     </row>
     <row r="21">
@@ -702,7 +702,7 @@
         </is>
       </c>
       <c r="C21" t="n">
-        <v>0.0001130891826266291</v>
+        <v>0.0001124974372270984</v>
       </c>
     </row>
     <row r="22">
@@ -715,7 +715,7 @@
         </is>
       </c>
       <c r="C22" t="n">
-        <v>9.092609189358801e-05</v>
+        <v>9.079747170250294e-05</v>
       </c>
     </row>
     <row r="23">
@@ -728,7 +728,7 @@
         </is>
       </c>
       <c r="C23" t="n">
-        <v>7.923502867468902e-05</v>
+        <v>7.868989601447069e-05</v>
       </c>
     </row>
     <row r="24">
@@ -741,33 +741,33 @@
         </is>
       </c>
       <c r="C24" t="n">
-        <v>7.849856502424525e-05</v>
+        <v>7.817307012744496e-05</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="1" t="n">
-        <v>26</v>
+        <v>7</v>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>type_3</t>
+          <t>(h$_{pq}$)$_{3}$</t>
         </is>
       </c>
       <c r="C25" t="n">
-        <v>6.332382366128924e-05</v>
+        <v>6.391886886259363e-05</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="1" t="n">
-        <v>7</v>
+        <v>26</v>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>(h$_{pq}$)$_{3}$</t>
+          <t>type_3</t>
         </is>
       </c>
       <c r="C26" t="n">
-        <v>6.229422531424987e-05</v>
+        <v>6.342866249886945e-05</v>
       </c>
     </row>
     <row r="27">
@@ -780,7 +780,7 @@
         </is>
       </c>
       <c r="C27" t="n">
-        <v>6.188937332518258e-05</v>
+        <v>6.213573282900078e-05</v>
       </c>
     </row>
     <row r="28">
@@ -793,7 +793,7 @@
         </is>
       </c>
       <c r="C28" t="n">
-        <v>6.064119789258407e-05</v>
+        <v>6.104371887992106e-05</v>
       </c>
     </row>
     <row r="29">
@@ -806,7 +806,7 @@
         </is>
       </c>
       <c r="C29" t="n">
-        <v>5.81142959577257e-05</v>
+        <v>5.905124198622398e-05</v>
       </c>
     </row>
     <row r="30">
@@ -819,7 +819,7 @@
         </is>
       </c>
       <c r="C30" t="n">
-        <v>5.677302013611078e-05</v>
+        <v>5.711014535110327e-05</v>
       </c>
     </row>
     <row r="31">
@@ -832,7 +832,7 @@
         </is>
       </c>
       <c r="C31" t="n">
-        <v>5.546368554742455e-05</v>
+        <v>5.662342197211688e-05</v>
       </c>
     </row>
     <row r="32">
@@ -845,7 +845,7 @@
         </is>
       </c>
       <c r="C32" t="n">
-        <v>5.407097440129359e-05</v>
+        <v>5.430566758509812e-05</v>
       </c>
     </row>
     <row r="33">
@@ -858,7 +858,7 @@
         </is>
       </c>
       <c r="C33" t="n">
-        <v>4.832877854486027e-05</v>
+        <v>4.772849392895252e-05</v>
       </c>
     </row>
     <row r="34">
@@ -871,7 +871,7 @@
         </is>
       </c>
       <c r="C34" t="n">
-        <v>4.63776751811166e-05</v>
+        <v>4.671264201576785e-05</v>
       </c>
     </row>
     <row r="35">
@@ -884,7 +884,7 @@
         </is>
       </c>
       <c r="C35" t="n">
-        <v>4.430305125644221e-05</v>
+        <v>4.349166215944893e-05</v>
       </c>
     </row>
     <row r="36">
@@ -897,7 +897,7 @@
         </is>
       </c>
       <c r="C36" t="n">
-        <v>4.351296597911749e-05</v>
+        <v>4.309329212750435e-05</v>
       </c>
     </row>
     <row r="37">
@@ -910,7 +910,7 @@
         </is>
       </c>
       <c r="C37" t="n">
-        <v>4.148963673576646e-05</v>
+        <v>4.110502705896857e-05</v>
       </c>
     </row>
     <row r="38">
@@ -923,7 +923,7 @@
         </is>
       </c>
       <c r="C38" t="n">
-        <v>3.890983984858438e-05</v>
+        <v>3.869533784731011e-05</v>
       </c>
     </row>
     <row r="39">
@@ -936,7 +936,7 @@
         </is>
       </c>
       <c r="C39" t="n">
-        <v>3.789906225436191e-05</v>
+        <v>3.788991975907304e-05</v>
       </c>
     </row>
     <row r="40">
@@ -949,7 +949,7 @@
         </is>
       </c>
       <c r="C40" t="n">
-        <v>3.76579489565839e-05</v>
+        <v>3.772976058511072e-05</v>
       </c>
     </row>
     <row r="41">
@@ -962,7 +962,7 @@
         </is>
       </c>
       <c r="C41" t="n">
-        <v>3.634887752271042e-05</v>
+        <v>3.705779891132885e-05</v>
       </c>
     </row>
     <row r="42">
@@ -975,7 +975,7 @@
         </is>
       </c>
       <c r="C42" t="n">
-        <v>3.609148909535752e-05</v>
+        <v>3.687477429133638e-05</v>
       </c>
     </row>
     <row r="43">
@@ -988,7 +988,7 @@
         </is>
       </c>
       <c r="C43" t="n">
-        <v>3.538520993210627e-05</v>
+        <v>3.576548924306131e-05</v>
       </c>
     </row>
     <row r="44">
@@ -1001,7 +1001,7 @@
         </is>
       </c>
       <c r="C44" t="n">
-        <v>3.461522469943708e-05</v>
+        <v>3.440180614521922e-05</v>
       </c>
     </row>
     <row r="45">
@@ -1014,7 +1014,7 @@
         </is>
       </c>
       <c r="C45" t="n">
-        <v>3.195172735559457e-05</v>
+        <v>3.260563657333214e-05</v>
       </c>
     </row>
     <row r="46">
@@ -1027,7 +1027,7 @@
         </is>
       </c>
       <c r="C46" t="n">
-        <v>3.130313721411322e-05</v>
+        <v>3.200731904606498e-05</v>
       </c>
     </row>
     <row r="47">
@@ -1040,7 +1040,7 @@
         </is>
       </c>
       <c r="C47" t="n">
-        <v>3.092636722056507e-05</v>
+        <v>3.107914340458499e-05</v>
       </c>
     </row>
     <row r="48">
@@ -1053,7 +1053,7 @@
         </is>
       </c>
       <c r="C48" t="n">
-        <v>3.043274911755724e-05</v>
+        <v>3.007818500800362e-05</v>
       </c>
     </row>
     <row r="49">
@@ -1066,33 +1066,33 @@
         </is>
       </c>
       <c r="C49" t="n">
-        <v>3.012612395866211e-05</v>
+        <v>2.996966448783539e-05</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" s="1" t="n">
-        <v>24</v>
+        <v>88</v>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>type_1</t>
+          <t>$(\langle pp \vert pp \rangle)_{2}$</t>
         </is>
       </c>
       <c r="C50" t="n">
-        <v>2.900498149893717e-05</v>
+        <v>2.879676746411079e-05</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" s="1" t="n">
-        <v>88</v>
+        <v>24</v>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>$(\langle pp \vert pp \rangle)_{2}$</t>
+          <t>type_1</t>
         </is>
       </c>
       <c r="C51" t="n">
-        <v>2.873174103310873e-05</v>
+        <v>2.855371418312209e-05</v>
       </c>
     </row>
     <row r="52">
@@ -1105,7 +1105,7 @@
         </is>
       </c>
       <c r="C52" t="n">
-        <v>2.735974874503543e-05</v>
+        <v>2.735543996812856e-05</v>
       </c>
     </row>
     <row r="53">
@@ -1118,7 +1118,7 @@
         </is>
       </c>
       <c r="C53" t="n">
-        <v>2.693695428614644e-05</v>
+        <v>2.667591872580024e-05</v>
       </c>
     </row>
     <row r="54">
@@ -1131,7 +1131,7 @@
         </is>
       </c>
       <c r="C54" t="n">
-        <v>2.660018404152719e-05</v>
+        <v>2.650735064875721e-05</v>
       </c>
     </row>
     <row r="55">
@@ -1144,7 +1144,7 @@
         </is>
       </c>
       <c r="C55" t="n">
-        <v>2.636309672595876e-05</v>
+        <v>2.649890117148161e-05</v>
       </c>
     </row>
     <row r="56">
@@ -1157,7 +1157,7 @@
         </is>
       </c>
       <c r="C56" t="n">
-        <v>2.627553051819163e-05</v>
+        <v>2.634583477723057e-05</v>
       </c>
     </row>
     <row r="57">
@@ -1170,7 +1170,7 @@
         </is>
       </c>
       <c r="C57" t="n">
-        <v>2.408600166531397e-05</v>
+        <v>2.561823773680406e-05</v>
       </c>
     </row>
     <row r="58">
@@ -1183,33 +1183,33 @@
         </is>
       </c>
       <c r="C58" t="n">
-        <v>2.279700504429114e-05</v>
+        <v>2.303693994883687e-05</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" s="1" t="n">
-        <v>84</v>
+        <v>77</v>
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>$(\langle rs\vert rs \rangle)_{1}$</t>
+          <t>$(\langle rs \vert sr \rangle)_{0}$</t>
         </is>
       </c>
       <c r="C59" t="n">
-        <v>2.250430427146552e-05</v>
+        <v>2.25048187751384e-05</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" s="1" t="n">
-        <v>77</v>
+        <v>84</v>
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>$(\langle rs \vert sr \rangle)_{0}$</t>
+          <t>$(\langle rs\vert rs \rangle)_{1}$</t>
         </is>
       </c>
       <c r="C60" t="n">
-        <v>2.237866494586781e-05</v>
+        <v>2.246514873551041e-05</v>
       </c>
     </row>
     <row r="61">
@@ -1222,7 +1222,7 @@
         </is>
       </c>
       <c r="C61" t="n">
-        <v>2.179926122061041e-05</v>
+        <v>2.187560378179541e-05</v>
       </c>
     </row>
     <row r="62">
@@ -1235,7 +1235,7 @@
         </is>
       </c>
       <c r="C62" t="n">
-        <v>2.082044498990063e-05</v>
+        <v>2.09321099499132e-05</v>
       </c>
     </row>
     <row r="63">
@@ -1248,33 +1248,33 @@
         </is>
       </c>
       <c r="C63" t="n">
-        <v>2.062428605721198e-05</v>
+        <v>2.07624467978136e-05</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" s="1" t="n">
-        <v>72</v>
+        <v>92</v>
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>$(\langle rr \vert rr \rangle)_{0}$</t>
+          <t>$(\langle rs\vert rs \rangle)_{2}$</t>
         </is>
       </c>
       <c r="C64" t="n">
-        <v>2.045364289483243e-05</v>
+        <v>2.048952420813167e-05</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" s="1" t="n">
-        <v>92</v>
+        <v>72</v>
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>$(\langle rs\vert rs \rangle)_{2}$</t>
+          <t>$(\langle rr \vert rr \rangle)_{0}$</t>
         </is>
       </c>
       <c r="C65" t="n">
-        <v>2.040265033973878e-05</v>
+        <v>2.037723893265321e-05</v>
       </c>
     </row>
     <row r="66">
@@ -1287,33 +1287,33 @@
         </is>
       </c>
       <c r="C66" t="n">
-        <v>1.87867814372272e-05</v>
+        <v>1.905354691654031e-05</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" s="1" t="n">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>$(\langle rr \vert rr \rangle)_{1}$</t>
+          <t>$(\langle pq \vert rs \rangle)_{1}$</t>
         </is>
       </c>
       <c r="C67" t="n">
-        <v>1.799005617505246e-05</v>
+        <v>1.780956549436204e-05</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" s="1" t="n">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>$(\langle pq \vert rs \rangle)_{1}$</t>
+          <t>$(\langle rr \vert rr \rangle)_{1}$</t>
         </is>
       </c>
       <c r="C68" t="n">
-        <v>1.772775365877889e-05</v>
+        <v>1.778838237289119e-05</v>
       </c>
     </row>
     <row r="69">
@@ -1326,7 +1326,7 @@
         </is>
       </c>
       <c r="C69" t="n">
-        <v>1.701504097703235e-05</v>
+        <v>1.713964518895558e-05</v>
       </c>
     </row>
     <row r="70">
@@ -1339,7 +1339,7 @@
         </is>
       </c>
       <c r="C70" t="n">
-        <v>1.627377193074433e-05</v>
+        <v>1.597476274801735e-05</v>
       </c>
     </row>
     <row r="71">
@@ -1352,7 +1352,7 @@
         </is>
       </c>
       <c r="C71" t="n">
-        <v>1.554449887350846e-05</v>
+        <v>1.570577278993051e-05</v>
       </c>
     </row>
     <row r="72">
@@ -1365,7 +1365,7 @@
         </is>
       </c>
       <c r="C72" t="n">
-        <v>1.482346234105408e-05</v>
+        <v>1.49319824293483e-05</v>
       </c>
     </row>
     <row r="73">
@@ -1378,7 +1378,7 @@
         </is>
       </c>
       <c r="C73" t="n">
-        <v>1.473497730149659e-05</v>
+        <v>1.471736703358423e-05</v>
       </c>
     </row>
     <row r="74">
@@ -1391,7 +1391,7 @@
         </is>
       </c>
       <c r="C74" t="n">
-        <v>1.417129867839537e-05</v>
+        <v>1.424630625450237e-05</v>
       </c>
     </row>
     <row r="75">
@@ -1404,7 +1404,7 @@
         </is>
       </c>
       <c r="C75" t="n">
-        <v>1.298961662338933e-05</v>
+        <v>1.299709986768325e-05</v>
       </c>
     </row>
     <row r="76">
@@ -1417,7 +1417,7 @@
         </is>
       </c>
       <c r="C76" t="n">
-        <v>1.276699542819349e-05</v>
+        <v>1.282684730540168e-05</v>
       </c>
     </row>
     <row r="77">
@@ -1430,7 +1430,7 @@
         </is>
       </c>
       <c r="C77" t="n">
-        <v>8.457505051443953e-06</v>
+        <v>8.570075516764712e-06</v>
       </c>
     </row>
     <row r="78">
@@ -1443,7 +1443,7 @@
         </is>
       </c>
       <c r="C78" t="n">
-        <v>7.69401841090897e-06</v>
+        <v>7.760604535262311e-06</v>
       </c>
     </row>
     <row r="79">
@@ -1456,7 +1456,7 @@
         </is>
       </c>
       <c r="C79" t="n">
-        <v>7.469141810934604e-06</v>
+        <v>7.56270922989295e-06</v>
       </c>
     </row>
     <row r="80">
@@ -1469,7 +1469,7 @@
         </is>
       </c>
       <c r="C80" t="n">
-        <v>6.682044303826883e-06</v>
+        <v>6.73564669488312e-06</v>
       </c>
     </row>
     <row r="81">
@@ -1482,7 +1482,7 @@
         </is>
       </c>
       <c r="C81" t="n">
-        <v>6.586494117822288e-06</v>
+        <v>6.636262760234857e-06</v>
       </c>
     </row>
     <row r="82">
@@ -1495,7 +1495,7 @@
         </is>
       </c>
       <c r="C82" t="n">
-        <v>5.704133493754906e-06</v>
+        <v>5.808940024011132e-06</v>
       </c>
     </row>
     <row r="83">
@@ -1508,7 +1508,7 @@
         </is>
       </c>
       <c r="C83" t="n">
-        <v>5.005483742455489e-06</v>
+        <v>4.972539675705066e-06</v>
       </c>
     </row>
     <row r="84">
@@ -1521,7 +1521,7 @@
         </is>
       </c>
       <c r="C84" t="n">
-        <v>3.516658677759995e-06</v>
+        <v>3.506727379004268e-06</v>
       </c>
     </row>
     <row r="85">
@@ -1534,7 +1534,7 @@
         </is>
       </c>
       <c r="C85" t="n">
-        <v>2.542959834740869e-06</v>
+        <v>2.534454001085589e-06</v>
       </c>
     </row>
     <row r="86">
@@ -1547,7 +1547,7 @@
         </is>
       </c>
       <c r="C86" t="n">
-        <v>1.983989184116141e-06</v>
+        <v>1.905792554111665e-06</v>
       </c>
     </row>
     <row r="87">
@@ -1560,7 +1560,7 @@
         </is>
       </c>
       <c r="C87" t="n">
-        <v>1.852283221776464e-06</v>
+        <v>1.837686862147749e-06</v>
       </c>
     </row>
     <row r="88">
@@ -1573,7 +1573,7 @@
         </is>
       </c>
       <c r="C88" t="n">
-        <v>1.567576123323096e-06</v>
+        <v>1.550880179602215e-06</v>
       </c>
     </row>
     <row r="89">
@@ -1586,7 +1586,7 @@
         </is>
       </c>
       <c r="C89" t="n">
-        <v>1.464956470240231e-06</v>
+        <v>1.455371227751058e-06</v>
       </c>
     </row>
     <row r="90">
@@ -1599,98 +1599,98 @@
         </is>
       </c>
       <c r="C90" t="n">
-        <v>1.049979491579088e-06</v>
+        <v>1.031986825824511e-06</v>
       </c>
     </row>
     <row r="91">
       <c r="A91" s="1" t="n">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="B91" t="inlineStr">
         <is>
-          <t>$(\langle pq \vert sr \rangle)_{0}$</t>
+          <t>$(\omega_{r})_{3}$</t>
         </is>
       </c>
       <c r="C91" t="n">
-        <v>3.48347419117156e-09</v>
+        <v>3.702886799327202e-09</v>
       </c>
     </row>
     <row r="92">
       <c r="A92" s="1" t="n">
-        <v>87</v>
+        <v>95</v>
       </c>
       <c r="B92" t="inlineStr">
         <is>
-          <t>$(\langle pq \vert sr \rangle)_{2}$</t>
+          <t>$(\langle pq \vert sr \rangle)_{3}$</t>
         </is>
       </c>
       <c r="C92" t="n">
-        <v>2.836982953050038e-09</v>
+        <v>2.349563757338587e-09</v>
       </c>
     </row>
     <row r="93">
       <c r="A93" s="1" t="n">
-        <v>49</v>
+        <v>87</v>
       </c>
       <c r="B93" t="inlineStr">
         <is>
-          <t>$(\omega_{r})_{1}$</t>
+          <t>$(\langle pq \vert sr \rangle)_{2}$</t>
         </is>
       </c>
       <c r="C93" t="n">
-        <v>1.445495406271398e-09</v>
+        <v>8.998001332837105e-10</v>
       </c>
     </row>
     <row r="94">
       <c r="A94" s="1" t="n">
-        <v>95</v>
+        <v>49</v>
       </c>
       <c r="B94" t="inlineStr">
         <is>
-          <t>$(\langle pq \vert sr \rangle)_{3}$</t>
+          <t>$(\omega_{r})_{1}$</t>
         </is>
       </c>
       <c r="C94" t="n">
-        <v>1.260694167268496e-09</v>
+        <v>7.551042994662785e-10</v>
       </c>
     </row>
     <row r="95">
       <c r="A95" s="1" t="n">
-        <v>41</v>
+        <v>79</v>
       </c>
       <c r="B95" t="inlineStr">
         <is>
-          <t>$\omega_{s}$</t>
+          <t>$(\langle pq \vert sr \rangle)_{1}$</t>
         </is>
       </c>
       <c r="C95" t="n">
-        <v>7.52823671623008e-10</v>
+        <v>5.907553279447355e-10</v>
       </c>
     </row>
     <row r="96">
       <c r="A96" s="1" t="n">
-        <v>37</v>
+        <v>57</v>
       </c>
       <c r="B96" t="inlineStr">
         <is>
-          <t>$(\omega_{r})_{0}$</t>
+          <t>$(\omega_{r})_{2}$</t>
         </is>
       </c>
       <c r="C96" t="n">
-        <v>7.46478408752709e-10</v>
+        <v>5.11256084297434e-10</v>
       </c>
     </row>
     <row r="97">
       <c r="A97" s="1" t="n">
-        <v>79</v>
+        <v>29</v>
       </c>
       <c r="B97" t="inlineStr">
         <is>
-          <t>$(\langle pq \vert sr \rangle)_{1}$</t>
+          <t>$(\omega_{p})_{0}$</t>
         </is>
       </c>
       <c r="C97" t="n">
-        <v>7.289108950573099e-10</v>
+        <v>2.297544444583153e-10</v>
       </c>
     </row>
     <row r="98">
@@ -1703,72 +1703,72 @@
         </is>
       </c>
       <c r="C98" t="n">
-        <v>5.556295352578441e-10</v>
+        <v>1.162309287639823e-10</v>
       </c>
     </row>
     <row r="99">
       <c r="A99" s="1" t="n">
-        <v>29</v>
+        <v>37</v>
       </c>
       <c r="B99" t="inlineStr">
         <is>
-          <t>$(\omega_{p})_{0}$</t>
+          <t>$(\omega_{r})_{0}$</t>
         </is>
       </c>
       <c r="C99" t="n">
-        <v>5.411192460754972e-10</v>
+        <v>1.096116241743758e-10</v>
       </c>
     </row>
     <row r="100">
       <c r="A100" s="1" t="n">
-        <v>57</v>
+        <v>41</v>
       </c>
       <c r="B100" t="inlineStr">
         <is>
-          <t>$(\omega_{r})_{2}$</t>
+          <t>$\omega_{s}$</t>
         </is>
       </c>
       <c r="C100" t="n">
-        <v>5.215721193317726e-10</v>
+        <v>5.811546438200716e-11</v>
       </c>
     </row>
     <row r="101">
       <c r="A101" s="1" t="n">
-        <v>65</v>
+        <v>45</v>
       </c>
       <c r="B101" t="inlineStr">
         <is>
-          <t>$(\omega_{r})_{3}$</t>
+          <t>$(\omega_{p})_{1}$</t>
         </is>
       </c>
       <c r="C101" t="n">
-        <v>3.036719385119349e-10</v>
+        <v>3.066411914505989e-11</v>
       </c>
     </row>
     <row r="102">
       <c r="A102" s="1" t="n">
-        <v>45</v>
+        <v>53</v>
       </c>
       <c r="B102" t="inlineStr">
         <is>
-          <t>$(\omega_{p})_{1}$</t>
+          <t>$(\omega_{p})_{2}$</t>
         </is>
       </c>
       <c r="C102" t="n">
-        <v>2.380755254404329e-10</v>
+        <v>2.083202989675856e-11</v>
       </c>
     </row>
     <row r="103">
       <c r="A103" s="1" t="n">
-        <v>53</v>
+        <v>69</v>
       </c>
       <c r="B103" t="inlineStr">
         <is>
-          <t>$(\omega_{p})_{2}$</t>
+          <t>$(\langle pq \vert sr \rangle)_{0}$</t>
         </is>
       </c>
       <c r="C103" t="n">
-        <v>7.958944058049979e-11</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>